<commit_message>
committed for matrix rotate
</commit_message>
<xml_diff>
--- a/bin/Algorithems_Tracking.xlsx
+++ b/bin/Algorithems_Tracking.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B37FD3-5FB8-4269-B591-AB5C2619BD0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -14,7 +13,7 @@
     <sheet name="Data Structure" sheetId="4" r:id="rId4"/>
     <sheet name="System Design" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="276">
   <si>
     <t>Core Java</t>
   </si>
@@ -949,7 +948,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1181,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1270,6 +1269,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1597,24 +1605,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:I52"/>
   <sheetViews>
     <sheetView topLeftCell="D24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="77.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="77.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1645,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1660,7 +1668,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1679,7 +1687,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1698,7 +1706,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1713,7 +1721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1730,7 +1738,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1747,7 +1755,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1764,7 +1772,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1781,7 +1789,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1796,7 +1804,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1817,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1822,7 +1830,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1835,7 +1843,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
         <v>18</v>
       </c>
@@ -1848,7 +1856,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1861,7 +1869,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
         <v>22</v>
       </c>
@@ -1874,7 +1882,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="6" t="s">
         <v>47</v>
       </c>
@@ -1887,7 +1895,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="6" t="s">
         <v>51</v>
       </c>
@@ -1900,7 +1908,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="6" t="s">
         <v>53</v>
       </c>
@@ -1913,7 +1921,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>206</v>
       </c>
@@ -1926,7 +1934,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>56</v>
       </c>
@@ -1939,7 +1947,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
         <v>63</v>
       </c>
@@ -1947,7 +1955,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="6" t="s">
         <v>153</v>
       </c>
@@ -1955,7 +1963,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>164</v>
       </c>
@@ -1963,127 +1971,127 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I28" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I29" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I30" s="6" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I31" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I32" s="17" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I36" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="6" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I43" s="6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I44" s="6" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I45" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I46" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I47" s="6" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I48" s="6" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I51" s="6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I52" s="31" t="s">
         <v>275</v>
       </c>
@@ -2095,20 +2103,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C1" s="23" t="s">
         <v>210</v>
       </c>
@@ -2116,7 +2124,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" s="17" t="s">
         <v>67</v>
       </c>
@@ -2124,7 +2132,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" s="17" t="s">
         <v>64</v>
       </c>
@@ -2132,7 +2140,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>165</v>
       </c>
@@ -2140,32 +2148,32 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="17" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>248</v>
       </c>
@@ -2177,138 +2185,138 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C3" s="34" t="s">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="37" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C4" s="34"/>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="37"/>
       <c r="D4" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C5" s="34"/>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="37"/>
       <c r="D5" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="34"/>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="37"/>
       <c r="D6" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C7" s="34"/>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="37"/>
       <c r="D7" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C8" s="34"/>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="37"/>
       <c r="D8" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C9" s="34"/>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="37"/>
       <c r="D9" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D12" s="16"/>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C13" s="34" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="37" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C14" s="34"/>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="37"/>
       <c r="D14" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" s="22" t="s">
         <v>216</v>
       </c>
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="22" t="s">
         <v>217</v>
       </c>
       <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="22" t="s">
         <v>218</v>
       </c>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
         <v>147</v>
       </c>
       <c r="D19" s="16"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="27" t="s">
         <v>274</v>
       </c>
       <c r="D20" s="16"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="21" t="s">
         <v>204</v>
       </c>
       <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="21" t="s">
         <v>205</v>
       </c>
@@ -2324,577 +2332,577 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D4" s="35" t="s">
+    <row r="3" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="38" t="s">
         <v>85</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D5" s="36"/>
-      <c r="E5" s="9" t="s">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="39"/>
+      <c r="E5" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D6" s="36"/>
-      <c r="E6" s="9" t="s">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="39"/>
+      <c r="E6" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="36"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D7" s="36"/>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="39"/>
       <c r="E7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="36"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D8" s="36"/>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="39"/>
       <c r="E8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D9" s="36"/>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="39"/>
       <c r="E9" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="G9" s="36"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D10" s="36"/>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="39"/>
       <c r="E10" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="36"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D11" s="36"/>
+    <row r="11" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="39"/>
       <c r="E11" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D12" s="36"/>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="39"/>
       <c r="E12" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D13" s="36"/>
+    <row r="13" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="39"/>
       <c r="E13" s="9" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D14" s="36"/>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="39"/>
       <c r="E14" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="38" t="s">
         <v>68</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D15" s="36"/>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="39"/>
       <c r="E15" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D16" s="36"/>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="39"/>
       <c r="E16" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="36"/>
+      <c r="G16" s="39"/>
       <c r="H16" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D17" s="36"/>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="39"/>
       <c r="E17" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D18" s="36"/>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="39"/>
       <c r="E18" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="36"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D19" s="36"/>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="39"/>
       <c r="E19" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G19" s="36"/>
+      <c r="G19" s="39"/>
       <c r="H19" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D20" s="36"/>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D20" s="39"/>
       <c r="E20" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="39"/>
       <c r="H20" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D21" s="37"/>
+    <row r="21" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="40"/>
       <c r="E21" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="37"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D25" s="35" t="s">
+    <row r="24" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="38" t="s">
         <v>102</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="G25" s="35" t="s">
+      <c r="G25" s="38" t="s">
         <v>111</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D26" s="36"/>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="39"/>
       <c r="E26" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="G26" s="36"/>
+      <c r="G26" s="39"/>
       <c r="H26" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D27" s="36"/>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="39"/>
       <c r="E27" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="G27" s="36"/>
+      <c r="G27" s="39"/>
       <c r="H27" s="9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D28" s="36"/>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="39"/>
       <c r="E28" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G28" s="36"/>
+      <c r="G28" s="39"/>
       <c r="H28" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D29" s="36"/>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="39"/>
       <c r="E29" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="G29" s="36"/>
+      <c r="G29" s="39"/>
       <c r="H29" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D30" s="36"/>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="39"/>
       <c r="E30" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G30" s="36"/>
+      <c r="G30" s="39"/>
       <c r="H30" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D31" s="36"/>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="39"/>
       <c r="E31" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="39"/>
       <c r="H31" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D32" s="36"/>
-      <c r="E32" s="9" t="s">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="39"/>
+      <c r="E32" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="G32" s="36"/>
+      <c r="G32" s="39"/>
       <c r="H32" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D33" s="36"/>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="39"/>
       <c r="E33" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G33" s="36"/>
+      <c r="G33" s="39"/>
       <c r="H33" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D34" s="36"/>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="39"/>
       <c r="E34" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="9" t="s">
+      <c r="G34" s="39"/>
+      <c r="H34" s="33" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D35" s="36"/>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D35" s="39"/>
       <c r="E35" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G35" s="36"/>
+      <c r="G35" s="39"/>
       <c r="H35" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D36" s="36"/>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D36" s="39"/>
       <c r="E36" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G36" s="36"/>
+      <c r="G36" s="39"/>
       <c r="H36" s="9" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D37" s="36"/>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D37" s="39"/>
       <c r="E37" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G37" s="36"/>
+      <c r="G37" s="39"/>
       <c r="H37" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D38" s="36"/>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D38" s="39"/>
       <c r="E38" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="36"/>
+      <c r="G38" s="39"/>
       <c r="H38" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D39" s="37"/>
+    <row r="39" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="40"/>
       <c r="E39" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="G39" s="37"/>
+      <c r="G39" s="40"/>
       <c r="H39" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D44" s="35" t="s">
+    <row r="43" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D44" s="38" t="s">
         <v>124</v>
       </c>
       <c r="E44" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="G44" s="35" t="s">
+      <c r="G44" s="38" t="s">
         <v>3</v>
       </c>
       <c r="H44" s="20" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D45" s="36"/>
+    <row r="45" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D45" s="39"/>
       <c r="E45" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="G45" s="36"/>
+      <c r="G45" s="39"/>
       <c r="H45" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D46" s="36"/>
+    <row r="46" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D46" s="39"/>
       <c r="E46" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="G46" s="36"/>
+      <c r="G46" s="39"/>
       <c r="H46" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D47" s="36"/>
-      <c r="E47" s="9" t="s">
+    <row r="47" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D47" s="39"/>
+      <c r="E47" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="G47" s="36"/>
+      <c r="G47" s="39"/>
       <c r="H47" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D48" s="36"/>
+    <row r="48" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D48" s="39"/>
       <c r="E48" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="G48" s="36"/>
+      <c r="G48" s="39"/>
       <c r="H48" s="12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D49" s="36"/>
-      <c r="E49" s="9" t="s">
+    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D49" s="39"/>
+      <c r="E49" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="G49" s="36"/>
+      <c r="G49" s="39"/>
       <c r="H49" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D50" s="36"/>
-      <c r="E50" s="9" t="s">
+    <row r="50" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D50" s="39"/>
+      <c r="E50" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="G50" s="36"/>
+      <c r="G50" s="39"/>
       <c r="H50" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D51" s="36"/>
-      <c r="E51" s="9" t="s">
+    <row r="51" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D51" s="39"/>
+      <c r="E51" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="G51" s="36"/>
+      <c r="G51" s="39"/>
       <c r="H51" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D52" s="36"/>
-      <c r="E52" s="9" t="s">
+    <row r="52" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D52" s="39"/>
+      <c r="E52" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="G52" s="36"/>
+      <c r="G52" s="39"/>
       <c r="H52" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D53" s="36"/>
-      <c r="E53" s="9" t="s">
+    <row r="53" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D53" s="39"/>
+      <c r="E53" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="G53" s="36"/>
+      <c r="G53" s="39"/>
       <c r="H53" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D54" s="36"/>
-      <c r="E54" s="9" t="s">
+    <row r="54" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D54" s="39"/>
+      <c r="E54" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="G54" s="36"/>
+      <c r="G54" s="39"/>
       <c r="H54" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D55" s="36"/>
-      <c r="E55" s="9" t="s">
+    <row r="55" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D55" s="39"/>
+      <c r="E55" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="G55" s="36"/>
+      <c r="G55" s="39"/>
       <c r="H55" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D56" s="36"/>
+    <row r="56" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D56" s="39"/>
       <c r="E56" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G56" s="36"/>
+      <c r="G56" s="39"/>
       <c r="H56" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D57" s="36"/>
-      <c r="E57" s="9" t="s">
+    <row r="57" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="39"/>
+      <c r="E57" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="G57" s="37"/>
+      <c r="G57" s="40"/>
       <c r="H57" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="4:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="D58" s="36"/>
-      <c r="E58" s="18" t="s">
+    <row r="58" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D58" s="39"/>
+      <c r="E58" s="35" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D59" s="36"/>
+    <row r="59" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D59" s="39"/>
       <c r="E59" s="18" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="60" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D60" s="36"/>
-      <c r="E60" s="9" t="s">
+    <row r="60" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="39"/>
+      <c r="E60" s="33" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D61" s="36"/>
-      <c r="E61" s="9" t="s">
+    <row r="61" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D61" s="39"/>
+      <c r="E61" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="G61" s="35" t="s">
+      <c r="G61" s="38" t="s">
         <v>200</v>
       </c>
       <c r="H61" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D62" s="36"/>
+    <row r="62" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D62" s="39"/>
       <c r="E62" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="G62" s="36"/>
-      <c r="H62" s="28" t="s">
+      <c r="G62" s="39"/>
+      <c r="H62" s="36" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="63" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D63" s="36"/>
+    <row r="63" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D63" s="39"/>
       <c r="E63" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="G63" s="36"/>
+      <c r="G63" s="39"/>
       <c r="H63" s="28" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="64" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D64" s="36"/>
+    <row r="64" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D64" s="39"/>
       <c r="E64" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="G64" s="36"/>
+      <c r="G64" s="39"/>
       <c r="H64" s="28" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D65" s="36"/>
-      <c r="E65" s="9" t="s">
+    <row r="65" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D65" s="39"/>
+      <c r="E65" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="G65" s="36"/>
-      <c r="H65" s="9" t="s">
+      <c r="G65" s="39"/>
+      <c r="H65" s="33" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="66" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D66" s="37"/>
+    <row r="66" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="40"/>
       <c r="E66" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="G66" s="37"/>
-      <c r="H66" s="10" t="s">
+      <c r="G66" s="40"/>
+      <c r="H66" s="34" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2915,21 +2923,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>222</v>
       </c>
@@ -2940,7 +2948,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
         <v>223</v>
       </c>
@@ -2951,7 +2959,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>224</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>225</v>
       </c>
@@ -2973,7 +2981,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>226</v>
       </c>
@@ -2984,7 +2992,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>227</v>
       </c>
@@ -2995,7 +3003,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>228</v>
       </c>
@@ -3003,7 +3011,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>229</v>
       </c>
@@ -3011,27 +3019,27 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>234</v>
       </c>

</xml_diff>